<commit_message>
last update create py files
</commit_message>
<xml_diff>
--- a/output1.xlsx
+++ b/output1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,7 +539,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>https://www.leguidedesmontres.com/en/products-new/a-lange-amp-sohne/1003/233021?PHPSESSID=2876fba59f16d0b8b9dbcf535948c460</t>
+          <t>https://www.leguidedesmontres.com/en/products-new/a-lange-amp-sohne/1003/233021?PHPSESSID=856f944be12372379eaf709910c4a801</t>
         </is>
       </c>
     </row>
@@ -592,241 +592,9 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>https://www.leguidedesmontres.com/en/products-new/a-lange-amp-sohne/1001/233025?PHPSESSID=2876fba59f16d0b8b9dbcf535948c460</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>h t t p s : / / w w w . l e g u i d e d e s m o n t r e s . c o m / _ f i l e s / r e f e r e n c e s / i m a g e s / 1 0 0 0 _ 1 0 4 3 _ a . _ l a n g e _ a m p _ s o h n e _ _ 2 3 3 . 0 3 2 . j p g</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>233.032</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>A. Lange &amp; Söhne</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Manual winding</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Hour, minute, second</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Pink gold</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Croco</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>ø 40,0mm</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>18,400.00 €</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>https://www.leguidedesmontres.com/en/products-new/a-lange-amp-sohne/1000/233032?PHPSESSID=2876fba59f16d0b8b9dbcf535948c460</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>h t t p s : / / w w w . l e g u i d e d e s m o n t r e s . c o m / _ f i l e s / r e f e r e n c e s / i m a g e s / 1 0 1 1 _ 1 0 5 5 _ a . _ l a n g e _ a m p _ s o h n e _ _ 4 0 2 . 0 3 2 . j p g</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>402.032</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>A. Lange &amp; Söhne</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>CHRONOGRAPHE</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Manual winding</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Hour, minute, second, chronograph flyback</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Pink gold</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Croco</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>ø 39,5mm</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>38,500.00 €</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>https://www.leguidedesmontres.com/en/products-new/a-lange-amp-sohne/1011/402032?PHPSESSID=2876fba59f16d0b8b9dbcf535948c460</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>h t t p s : / / w w w . l e g u i d e d e s m o n t r e s . c o m / _ f i l e s / r e f e r e n c e s / i m a g e s / 1 0 0 8 _ 1 0 5 2 _ a . _ l a n g e _ a m p _ s o h n e _ _ 4 0 2 . 0 2 6 . j p g</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>402.026</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>A. Lange &amp; Söhne</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>CHRONOGRAPHE</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Manual winding</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Hour, minute, second, chronograph flyback</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Or blanc</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Croco</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>ø 39,5mm</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>39,500.00 €</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>https://www.leguidedesmontres.com/en/products-new/a-lange-amp-sohne/1008/402026?PHPSESSID=2876fba59f16d0b8b9dbcf535948c460</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
+          <t>https://www.leguidedesmontres.com/en/products-new/a-lange-amp-sohne/1001/233025?PHPSESSID=856f944be12372379eaf709910c4a801</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>